<commit_message>
added comments and help, modified code
</commit_message>
<xml_diff>
--- a/training and detection/att.xlsx
+++ b/training and detection/att.xlsx
@@ -374,7 +374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A3:C90"/>
+  <dimension ref="A3:C100"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
@@ -1342,59 +1342,177 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>26/02/2019</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>26/02/2019</t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="inlineStr">
         <is>
           <t>21:22:24</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Sno</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Sno</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="inlineStr">
         <is>
           <t>Present</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
-        <v>1</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>shamil</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
+      <c r="A89" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t>shamil</t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>2</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>abhi</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
+      <c r="A90" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>abhi</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>26/04/2019</t>
+        </is>
+      </c>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>02:48:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>Sno</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B94" s="1" t="inlineStr">
+        <is>
+          <t>abhi</t>
+        </is>
+      </c>
+      <c r="C94" s="1" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B95" s="1" t="inlineStr">
+        <is>
+          <t>shamil</t>
+        </is>
+      </c>
+      <c r="C95" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>26/04/2019</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>02:52:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Sno</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>1</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>abhi</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>2</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>shamil</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
         <is>
           <t>no</t>
         </is>

</xml_diff>